<commit_message>
rutas y correos especificos con toda la data
</commit_message>
<xml_diff>
--- a/Rosember/Scripts Miguel/Enviar_correos_mapas/correos.xlsx
+++ b/Rosember/Scripts Miguel/Enviar_correos_mapas/correos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Geodata\Mapas_Despoblacion\Scripts Miguel\Enviar_correos_mapas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD11561A-3617-4B34-9B6A-A064CFCE65BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{627651F9-B3A0-4CF9-8503-2F3F5000CDF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{ADC469B3-F03B-4F24-B9A9-82F7E2D85450}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{ADC469B3-F03B-4F24-B9A9-82F7E2D85450}"/>
   </bookViews>
   <sheets>
     <sheet name="Propias" sheetId="1" r:id="rId1"/>
@@ -334,9 +334,6 @@
     <t>ammartinez@incauca.com; lsaavedra@incauca.com</t>
   </si>
   <si>
-    <t>Julian Andres Pena Ospina &lt;japenao@incauca.com&gt;; Roider Carabali Mezu &lt;rcarabali@incauca.com&gt;; Ginna Constanza Rosero Arevalo &lt;gcrosero@incauca.com&gt;; Félix Andrés  Molina Serrano &lt;famolina@incauca.com&gt;; Aderson Orozco Gonzalez &lt;aorozco@incauca.com&gt;; Edwin Fabian Mesias &lt;efmesias@incauca.com&gt;</t>
-  </si>
-  <si>
     <t xml:space="preserve">
 Buenos día.
 En Incauca estamos optimizando las labores de campo y cosecha mediante el uso de fotografías aéreas con Drone de alto detalle para determinar lo siguiente (ver documento pdf adjunto):
@@ -361,12 +358,15 @@
 APP: https://drive.google.com/file/d/11eCmqAVLjRybm7imDJpu_rn_qX3Pm5yb/view?usp=drive_link  
 Quedo atento, cordialmente, Rosemberg moreno</t>
   </si>
+  <si>
+    <t>Julian Andres Pena Ospina &lt;japenao@incauca.com&gt;; Ginna Constanza Rosero Arevalo &lt;gcrosero@incauca.com&gt;; Félix Andrés  Molina Serrano &lt;famolina@incauca.com&gt;; Aderson Orozco Gonzalez &lt;aorozco@incauca.com&gt;; Edwin Fabian Mesias &lt;efmesias@incauca.com&gt;</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -407,6 +407,14 @@
     </font>
     <font>
       <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -475,7 +483,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -522,6 +530,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -541,9 +550,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -581,7 +590,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -687,7 +696,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -829,7 +838,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -887,7 +896,7 @@
         <v>12</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -904,7 +913,7 @@
         <v>10</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -921,7 +930,7 @@
         <v>8</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -938,7 +947,7 @@
         <v>6</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -955,7 +964,7 @@
         <v>4</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -972,7 +981,7 @@
         <v>2</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -989,7 +998,7 @@
         <v>0</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1003,10 +1012,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F74CFDD4-1611-4438-AFAF-588B93229D40}">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1019,7 +1028,7 @@
     <col min="6" max="6" width="25.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>89</v>
       </c>
@@ -1039,7 +1048,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>20</v>
       </c>
@@ -1050,17 +1059,17 @@
         <v>48</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E2" s="16" t="str">
         <f>"Mapas resiembra "&amp;B2&amp;""</f>
         <v>Mapas resiembra JIGUAL</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>21</v>
       </c>
@@ -1071,17 +1080,17 @@
         <v>49</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E3" s="16" t="str">
         <f t="shared" ref="E3:E29" si="0">"Mapas resiembra "&amp;B3&amp;""</f>
         <v>Mapas resiembra MEXICO</v>
       </c>
       <c r="F3" s="17" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>22</v>
       </c>
@@ -1092,17 +1101,17 @@
         <v>50</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E4" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Mapas resiembra GUAYABITAL</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>23</v>
       </c>
@@ -1113,17 +1122,18 @@
         <v>50</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E5" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Mapas resiembra LA COMUNIDAD</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+      <c r="J5" s="18"/>
+    </row>
+    <row r="6" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>24</v>
       </c>
@@ -1134,17 +1144,17 @@
         <v>50</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E6" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Mapas resiembra SANTAGRO</v>
       </c>
       <c r="F6" s="17" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>25</v>
       </c>
@@ -1155,17 +1165,17 @@
         <v>51</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E7" s="16" t="str">
         <f t="shared" si="0"/>
         <v>Mapas resiembra CANADA - SANINT</v>
       </c>
       <c r="F7" s="17" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>26</v>
       </c>
@@ -1176,17 +1186,17 @@
         <v>51</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E8" s="16" t="str">
         <f t="shared" si="0"/>
         <v>Mapas resiembra EL SOCORRO</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>27</v>
       </c>
@@ -1197,17 +1207,17 @@
         <v>51</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E9" s="16" t="str">
         <f t="shared" si="0"/>
         <v>Mapas resiembra GUACAMAYAS</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>28</v>
       </c>
@@ -1218,17 +1228,17 @@
         <v>51</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E10" s="16" t="str">
         <f t="shared" si="0"/>
         <v>Mapas resiembra JUDEA SANINT</v>
       </c>
       <c r="F10" s="17" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>29</v>
       </c>
@@ -1239,17 +1249,17 @@
         <v>51</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E11" s="16" t="str">
         <f t="shared" si="0"/>
         <v>Mapas resiembra LA ARGENTINA</v>
       </c>
       <c r="F11" s="17" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>30</v>
       </c>
@@ -1260,17 +1270,17 @@
         <v>51</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E12" s="16" t="str">
         <f t="shared" si="0"/>
         <v>Mapas resiembra LA MARAVILLOSA</v>
       </c>
       <c r="F12" s="17" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>31</v>
       </c>
@@ -1281,17 +1291,17 @@
         <v>51</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E13" s="16" t="str">
         <f t="shared" si="0"/>
         <v>Mapas resiembra PERICO NEGRO</v>
       </c>
       <c r="F13" s="17" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>32</v>
       </c>
@@ -1302,17 +1312,17 @@
         <v>52</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E14" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Mapas resiembra EL CENIT</v>
       </c>
       <c r="F14" s="17" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>33</v>
       </c>
@@ -1323,17 +1333,17 @@
         <v>52</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E15" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Mapas resiembra EL LAGO</v>
       </c>
       <c r="F15" s="17" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>34</v>
       </c>
@@ -1344,14 +1354,14 @@
         <v>53</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E16" s="16" t="str">
         <f t="shared" si="0"/>
         <v>Mapas resiembra JAPIO NO.2</v>
       </c>
       <c r="F16" s="17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1365,14 +1375,14 @@
         <v>53</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E17" s="16" t="str">
         <f t="shared" si="0"/>
         <v>Mapas resiembra JAPIO TRES</v>
       </c>
       <c r="F17" s="17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1386,14 +1396,14 @@
         <v>54</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E18" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Mapas resiembra EL CASTILLO</v>
       </c>
       <c r="F18" s="17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1407,14 +1417,14 @@
         <v>55</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E19" s="16" t="str">
         <f t="shared" si="0"/>
         <v>Mapas resiembra EL COROZO</v>
       </c>
       <c r="F19" s="17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1428,14 +1438,14 @@
         <v>56</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E20" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Mapas resiembra EL CONGO -   MACHIN</v>
       </c>
       <c r="F20" s="17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1449,14 +1459,14 @@
         <v>57</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E21" s="16" t="str">
         <f t="shared" si="0"/>
         <v>Mapas resiembra LA REGINA</v>
       </c>
       <c r="F21" s="17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1470,14 +1480,14 @@
         <v>58</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E22" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Mapas resiembra CONFIN BARRIOS</v>
       </c>
       <c r="F22" s="17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1491,14 +1501,14 @@
         <v>58</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E23" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Mapas resiembra GUAIRA BARRIOS</v>
       </c>
       <c r="F23" s="17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1512,14 +1522,14 @@
         <v>58</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E24" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Mapas resiembra LA CILIA</v>
       </c>
       <c r="F24" s="17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1533,14 +1543,14 @@
         <v>58</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E25" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Mapas resiembra PATIO BONITO BARRIOS</v>
       </c>
       <c r="F25" s="17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1554,14 +1564,14 @@
         <v>58</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E26" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Mapas resiembra SILENCIO BARRIOS</v>
       </c>
       <c r="F26" s="17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1575,14 +1585,14 @@
         <v>59</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E27" s="16" t="str">
         <f t="shared" si="0"/>
         <v>Mapas resiembra LA CAMELIA</v>
       </c>
       <c r="F27" s="17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1596,14 +1606,14 @@
         <v>60</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E28" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Mapas resiembra EL GRAMAL</v>
       </c>
       <c r="F28" s="17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1617,14 +1627,14 @@
         <v>60</v>
       </c>
       <c r="D29" s="15" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E29" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Mapas resiembra LA INDIA</v>
       </c>
       <c r="F29" s="17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>